<commit_message>
chore: Add LY3 data file.
</commit_message>
<xml_diff>
--- a/src/data/ly3.xlsx
+++ b/src/data/ly3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -47,6 +47,24 @@
   <si>
     <t xml:space="preserve">Image</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">蔬苑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Idaten garden</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -56,7 +74,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -77,6 +95,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +156,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,6 +179,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -281,7 +313,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H86" activeCellId="1" sqref="A1:H1 H86"/>
+      <selection pane="bottomLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -961,7 +993,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1:H1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,15 +1665,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1665,6 +1697,14 @@
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Set `Show` column to `true`.
</commit_message>
<xml_diff>
--- a/src/data/ly3.xlsx
+++ b/src/data/ly3.xlsx
@@ -53,6 +53,7 @@
         <sz val="10"/>
         <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">蔬苑</t>
     </r>
@@ -70,7 +71,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">中国福建沙县小吃
@@ -81,6 +82,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Fujian Shaxian snacks </t>
     </r>
@@ -89,7 +91,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">一碟一味 </t>
@@ -99,6 +101,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">One Plate, One Flavour</t>
     </r>
@@ -109,6 +112,7 @@
         <sz val="10"/>
         <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">我想吃 </t>
     </r>
@@ -126,7 +130,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">食</t>
@@ -136,13 +140,14 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">园</t>
@@ -152,7 +157,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">好料 </t>
@@ -162,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">HAOLIU</t>
     </r>
@@ -170,7 +176,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">生活银座 </t>
@@ -180,6 +186,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Living Ginza Sushi &amp; Bento</t>
     </r>
@@ -188,7 +195,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">一口云 </t>
@@ -198,6 +205,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">YIKOU YUN</t>
     </r>
@@ -206,7 +214,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">兰州拉面</t>
@@ -216,6 +224,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Lanzhou Ramen</t>
     </r>
@@ -224,7 +233,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">香遇时光 </t>
@@ -234,6 +243,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Blissful Moments</t>
     </r>
@@ -242,7 +252,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">芋时光 </t>
@@ -252,6 +262,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">YU Moments</t>
     </r>
@@ -260,7 +271,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">恋恋不忘 </t>
@@ -270,6 +281,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RASA SAYANG</t>
     </r>
@@ -281,7 +293,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">点点点</t>
@@ -306,7 +318,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">蒂蒂果（果汁</t>
@@ -323,7 +335,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">切果</t>
@@ -351,7 +363,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">爆汁炸鸡堡</t>
@@ -364,7 +376,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">食惠烧烤涮</t>
@@ -383,7 +395,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">一口甜</t>
@@ -400,7 +412,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">烘焙</t>
@@ -419,7 +431,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">榴宝贝</t>
@@ -429,7 +441,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天猫咖啡</t>
@@ -439,6 +451,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/Tmall Coffee</t>
     </r>
@@ -447,7 +460,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">千叶</t>
@@ -466,7 +479,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
+        <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">韩屋村 </t>
@@ -486,11 +499,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -516,6 +530,7 @@
       <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -525,13 +540,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="DejaVu Sans"/>
+      <name val="LXGW WenKai Mono"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -583,7 +593,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -612,23 +622,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,7 +766,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
+      <selection pane="bottomLeft" activeCell="H86" activeCellId="1" sqref="F2:F34 H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1440,7 +1446,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="F2:F34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2115,14 +2121,14 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2152,146 +2158,261 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="F2" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="F4" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="F5" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="3" t="n">
         <v>4</v>
+      </c>
+      <c r="F7" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="F11" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="F12" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="F14" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="F16" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="F18" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="F19" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="F20" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="F21" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="F22" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="F23" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="F24" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="F25" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>25</v>
+      </c>
+      <c r="F26" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="F27" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="F28" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="F29" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>29</v>
+      </c>
+      <c r="F30" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="F31" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="F33" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="F34" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:Update ly3.xlsx about DDD
</commit_message>
<xml_diff>
--- a/src/data/ly3.xlsx
+++ b/src/data/ly3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AED6E7F-E4D2-4086-8511-44E3AAA270F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09108F0C-68B1-49CF-B705-BE6338CDB05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -606,6 +606,14 @@
   </si>
   <si>
     <t>sun</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDD</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddd</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2267,8 +2275,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -2433,6 +2441,15 @@
       </c>
     </row>
     <row r="13" spans="1:8">
+      <c r="A13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F13" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>

</xml_diff>

<commit_message>
fix: Remove or hide some unavailable stores.
</commit_message>
<xml_diff>
--- a/src/data/ly3.xlsx
+++ b/src/data/ly3.xlsx
@@ -1,35 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09108F0C-68B1-49CF-B705-BE6338CDB05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
-    <sheet name="1" sheetId="2" r:id="rId2"/>
-    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="1" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="2" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -38,39 +22,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>3E</t>
-  </si>
-  <si>
-    <t>daily_necessity</t>
-  </si>
-  <si>
-    <t>3e</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily_necessity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e</t>
   </si>
   <si>
     <r>
@@ -90,26 +74,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>中闽美食</t>
-    </r>
-  </si>
-  <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>zhongmin</t>
-  </si>
-  <si>
-    <t>Bean's Express</t>
-  </si>
-  <si>
-    <t>bean</t>
-  </si>
-  <si>
-    <t>Mad Plate Express</t>
-  </si>
-  <si>
-    <t>mad</t>
+      <t xml:space="preserve">中闽美食</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zhongmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean's Express</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mad Plate Express</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mad</t>
   </si>
   <si>
     <r>
@@ -119,7 +103,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Xiao Jiu Zho</t>
+      <t xml:space="preserve">Xiao Jiu Zho</t>
     </r>
     <r>
       <rPr>
@@ -128,7 +112,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>小九州</t>
+      <t xml:space="preserve">小九州</t>
     </r>
   </si>
   <si>
@@ -149,11 +133,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>膳一城</t>
-    </r>
-  </si>
-  <si>
-    <t>castle</t>
+      <t xml:space="preserve">膳一城</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">castle</t>
   </si>
   <si>
     <r>
@@ -173,17 +157,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>槟城风味</t>
-    </r>
-  </si>
-  <si>
-    <t>penang</t>
-  </si>
-  <si>
-    <t>Kami Cemerlang</t>
-  </si>
-  <si>
-    <t>kami</t>
+      <t xml:space="preserve">槟城风味</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">penang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kami Cemerlang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kami</t>
   </si>
   <si>
     <r>
@@ -203,11 +187,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>中国穆斯林小炒</t>
-    </r>
-  </si>
-  <si>
-    <t>takwa</t>
+      <t xml:space="preserve">中国穆斯林小炒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">takwa</t>
   </si>
   <si>
     <r>
@@ -227,11 +211,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>有你香锅</t>
-    </r>
-  </si>
-  <si>
-    <t>hotpot</t>
+      <t xml:space="preserve">有你香锅</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">hotpot</t>
   </si>
   <si>
     <r>
@@ -251,7 +235,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>食</t>
+      <t xml:space="preserve">食</t>
     </r>
     <r>
       <rPr>
@@ -260,7 +244,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>.</t>
+      <t xml:space="preserve">.</t>
     </r>
     <r>
       <rPr>
@@ -269,35 +253,11 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>园</t>
-    </r>
-  </si>
-  <si>
-    <t>shiyuan</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">I Want To Eat
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>我想吃</t>
-    </r>
-  </si>
-  <si>
-    <t>eat</t>
+      <t xml:space="preserve">园</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">shiyuan</t>
   </si>
   <si>
     <r>
@@ -307,7 +267,71 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">One Plate, One Flavour
+      <t xml:space="preserve">Shaxian snacks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">沙县小吃 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">shaxian-ly3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Idaten garden
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">臻蔬福</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">snack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MALATANG AND NOODLES
+孙小野 麻辣烫香锅家乡面馆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RASA SAYANG
 </t>
     </r>
     <r>
@@ -317,11 +341,18 @@
         <family val="1"/>
         <charset val="134"/>
       </rPr>
-      <t>一碟一味</t>
-    </r>
-  </si>
-  <si>
-    <t>plate</t>
+      <t xml:space="preserve">恋恋不忘</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blissful Moments
+香遇时光 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blissful</t>
   </si>
   <si>
     <r>
@@ -331,61 +362,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Shaxian snacks
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">沙县小吃 </t>
-    </r>
-  </si>
-  <si>
-    <t>shaxian-ly3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Idaten garden
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-      </rPr>
-      <t>臻蔬福</t>
-    </r>
-  </si>
-  <si>
-    <t>snack</t>
-  </si>
-  <si>
-    <t>garden</t>
-  </si>
-  <si>
-    <t>MALATANG AND NOODLES
-孙小野 麻辣烫香锅家乡面馆</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">RASA SAYANG
+      <t xml:space="preserve">YU Moments
 </t>
     </r>
     <r>
@@ -395,20 +372,22 @@
         <family val="1"/>
         <charset val="134"/>
       </rPr>
-      <t>恋恋不忘</t>
-    </r>
-  </si>
-  <si>
-    <t>rasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blissful Moments
-香遇时光 </t>
-  </si>
-  <si>
-    <t>blissful</t>
-  </si>
-  <si>
+      <t xml:space="preserve">芋时光</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">yu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">兰州拉面</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -416,21 +395,62 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">YU Moments
-</t>
+      <t xml:space="preserve">Lanzhou Ramen</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">lanzhou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YIKOU YUN
+一口云</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Living Ginza Sushi &amp; Bento
+生活银座</t>
+  </si>
+  <si>
+    <t xml:space="preserve">living</t>
+  </si>
+  <si>
+    <t xml:space="preserve">houliu
+好料</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haoliu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmall Coffee
+天猫咖啡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmall</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Durian Baby </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="LXGW WenKai Mono"/>
-        <family val="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>芋时光</t>
-    </r>
-  </si>
-  <si>
-    <t>yu</t>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">榴宝贝</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">durian</t>
   </si>
   <si>
     <r>
@@ -440,43 +460,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>兰州拉面</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Lanzhou Ramen</t>
-    </r>
-  </si>
-  <si>
-    <t>lanzhou</t>
-  </si>
-  <si>
-    <t>YIKOU YUN
-一口云</t>
-  </si>
-  <si>
-    <t>yun</t>
-  </si>
-  <si>
-    <t>Living Ginza Sushi &amp; Bento
-生活银座</t>
-  </si>
-  <si>
-    <t>living</t>
-  </si>
-  <si>
-    <t>houliu
-好料</t>
-  </si>
-  <si>
-    <t>haoliu</t>
-  </si>
-  <si>
+      <t xml:space="preserve">一口甜</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -484,7 +469,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Durian Baby </t>
+      <t xml:space="preserve">.</t>
     </r>
     <r>
       <rPr>
@@ -493,50 +478,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>榴宝贝</t>
-    </r>
-  </si>
-  <si>
-    <t>durian</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>一口甜</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>烘焙</t>
-    </r>
-  </si>
-  <si>
-    <t>yikou</t>
-  </si>
-  <si>
-    <t>Tmall Coffee
-天猫咖啡</t>
-  </si>
-  <si>
-    <t>tmall</t>
+      <t xml:space="preserve">烘焙</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">yikou</t>
   </si>
   <si>
     <r>
@@ -556,11 +502,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>爆汁炸鸡堡</t>
-    </r>
-  </si>
-  <si>
-    <t>boom</t>
+      <t xml:space="preserve">爆汁炸鸡堡</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">boom</t>
   </si>
   <si>
     <r>
@@ -570,7 +516,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>蒂蒂果（果汁</t>
+      <t xml:space="preserve">蒂蒂果（果汁</t>
     </r>
     <r>
       <rPr>
@@ -579,7 +525,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>&amp;</t>
+      <t xml:space="preserve">&amp;</t>
     </r>
     <r>
       <rPr>
@@ -588,7 +534,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>切果</t>
+      <t xml:space="preserve">切果</t>
     </r>
     <r>
       <rPr>
@@ -597,39 +543,44 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>)
+      <t xml:space="preserve">)
 DEE Fruit &amp; Juice</t>
     </r>
   </si>
   <si>
-    <t>dee</t>
-  </si>
-  <si>
-    <t>sun</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>DDD</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddd</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <t xml:space="preserve">dee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -659,23 +610,12 @@
       <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="1"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="LXGW WenKai Mono"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -688,146 +628,170 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="15">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -880,29 +844,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" style="1"/>
-    <col min="3" max="3" width="11.54296875" style="2"/>
-    <col min="4" max="6" width="11.54296875" style="1"/>
-    <col min="11" max="16384" width="11.54296875" style="3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -928,7 +894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="35.25" customHeight="1">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -938,13 +904,13 @@
       <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -952,7 +918,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -960,7 +926,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -968,7 +934,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1">
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -976,7 +942,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -984,7 +950,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -992,7 +958,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1000,7 +966,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="35.25" customHeight="1">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1008,7 +974,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="35.25" customHeight="1">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1016,7 +982,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="35.25" customHeight="1">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1024,7 +990,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="35.25" customHeight="1">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1032,7 +998,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1040,7 +1006,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1048,7 +1014,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1056,7 +1022,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="35.25" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1064,7 +1030,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="35.25" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1072,7 +1038,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="35.25" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1080,7 +1046,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="35.25" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1088,7 +1054,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="35.25" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1096,7 +1062,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="35.25" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1104,7 +1070,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="35.25" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1112,7 +1078,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="35.25" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1120,7 +1086,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="35.25" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1128,7 +1094,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="35.25" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1136,7 +1102,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="35.25" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1144,7 +1110,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="35.25" customHeight="1">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1152,7 +1118,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="35.25" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1160,7 +1126,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" ht="35.25" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1168,7 +1134,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" ht="35.25" customHeight="1">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1176,7 +1142,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" ht="35.25" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1184,7 +1150,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="35.25" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1192,7 +1158,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" ht="35.25" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1200,7 +1166,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="35.25" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1208,7 +1174,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" ht="35.25" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1216,7 +1182,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="35.25" customHeight="1">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1224,7 +1190,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" ht="35.25" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1232,7 +1198,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" ht="35.25" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1240,7 +1206,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" ht="35.25" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1248,7 +1214,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="35.25" customHeight="1">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1256,7 +1222,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="35.25" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1264,7 +1230,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" ht="35.25" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1272,7 +1238,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" ht="35.25" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1280,7 +1246,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="35.25" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1288,7 +1254,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" ht="35.25" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1296,7 +1262,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="35.25" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1304,7 +1270,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="35.25" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1312,7 +1278,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="35.25" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1320,7 +1286,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="35.25" customHeight="1">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1328,7 +1294,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="35.25" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1336,7 +1302,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="35.25" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1344,7 +1310,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" ht="35.25" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1352,7 +1318,7 @@
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" ht="35.25" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1360,7 +1326,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" ht="35.25" customHeight="1">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1368,7 +1334,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" ht="35.25" customHeight="1">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1376,7 +1342,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" ht="35.25" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1384,7 +1350,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" ht="35.25" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1392,7 +1358,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" ht="35.25" customHeight="1">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1400,7 +1366,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" ht="35.25" customHeight="1">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1408,7 +1374,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" ht="35.25" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1416,7 +1382,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" ht="35.25" customHeight="1">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1424,7 +1390,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" ht="35.25" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1432,7 +1398,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" ht="35.25" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1440,7 +1406,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" ht="35.25" customHeight="1">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1448,7 +1414,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" ht="35.25" customHeight="1">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1456,7 +1422,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" ht="35.25" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1464,7 +1430,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" ht="35.25" customHeight="1">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1472,7 +1438,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" ht="35.25" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1480,7 +1446,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" ht="35.25" customHeight="1">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1488,7 +1454,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" ht="35.25" customHeight="1">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1496,7 +1462,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" ht="35.25" customHeight="1">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1504,7 +1470,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" ht="35.25" customHeight="1">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1512,7 +1478,7 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" ht="35.25" customHeight="1">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1520,7 +1486,7 @@
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" ht="35.25" customHeight="1">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1528,7 +1494,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" ht="35.25" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1536,7 +1502,7 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" ht="35.25" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1544,7 +1510,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" ht="35.25" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1553,16 +1519,16 @@
       <c r="F78" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B1002" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1570,21 +1536,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="11.54296875" style="3"/>
-    <col min="7" max="16384" width="11.54296875" style="7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="3" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="7" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="35.25" customHeight="1">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -1624,7 +1594,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1608,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -1652,21 +1622,21 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="8" t="n">
         <v>9</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1">
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -1680,7 +1650,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
@@ -1694,7 +1664,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1708,7 +1678,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -1722,7 +1692,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="35.25" customHeight="1">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1736,47 +1706,47 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:8" ht="35.25" customHeight="1">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="35.25" customHeight="1">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="35.25" customHeight="1">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" ht="35.25" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="35.25" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" ht="35.25" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1784,12 +1754,12 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="35.25" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" ht="35.25" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1797,7 +1767,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" ht="35.25" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1805,7 +1775,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="35.25" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1813,7 +1783,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" ht="35.25" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1821,7 +1791,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="35.25" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1829,7 +1799,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" ht="35.25" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1837,7 +1807,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="35.25" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1845,7 +1815,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" ht="35.25" customHeight="1">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1853,7 +1823,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" ht="35.25" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1861,7 +1831,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" ht="35.25" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1869,7 +1839,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="35.25" customHeight="1">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1877,7 +1847,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="35.25" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1885,7 +1855,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="35.25" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1893,7 +1863,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="35.25" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1901,7 +1871,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" ht="35.25" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1909,7 +1879,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="35.25" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1917,7 +1887,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" ht="35.25" customHeight="1">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1925,7 +1895,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" ht="35.25" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1933,7 +1903,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" ht="35.25" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1941,7 +1911,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="35.25" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1949,7 +1919,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" ht="35.25" customHeight="1">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1957,7 +1927,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="35.25" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1965,7 +1935,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="35.25" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -1973,7 +1943,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" ht="35.25" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1981,7 +1951,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="35.25" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1989,7 +1959,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" ht="35.25" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -1997,7 +1967,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="35.25" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -2005,7 +1975,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="35.25" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2013,7 +1983,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" ht="35.25" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -2021,7 +1991,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" ht="35.25" customHeight="1">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -2029,7 +1999,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" ht="35.25" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -2037,7 +2007,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" ht="35.25" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -2045,7 +2015,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" ht="35.25" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -2053,7 +2023,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" ht="35.25" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -2061,7 +2031,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
     </row>
-    <row r="55" spans="1:6" ht="35.25" customHeight="1">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -2069,7 +2039,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
     </row>
-    <row r="56" spans="1:6" ht="35.25" customHeight="1">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -2077,7 +2047,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
     </row>
-    <row r="57" spans="1:6" ht="35.25" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -2085,7 +2055,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="1:6" ht="35.25" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -2093,7 +2063,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
     </row>
-    <row r="59" spans="1:6" ht="35.25" customHeight="1">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -2101,7 +2071,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" ht="35.25" customHeight="1">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -2109,7 +2079,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" ht="35.25" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -2117,7 +2087,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
     </row>
-    <row r="62" spans="1:6" ht="35.25" customHeight="1">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -2125,7 +2095,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
     </row>
-    <row r="63" spans="1:6" ht="35.25" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -2133,7 +2103,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
     </row>
-    <row r="64" spans="1:6" ht="35.25" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -2141,7 +2111,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
     </row>
-    <row r="65" spans="1:6" ht="35.25" customHeight="1">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -2149,7 +2119,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
     </row>
-    <row r="66" spans="1:6" ht="35.25" customHeight="1">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -2157,7 +2127,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
     </row>
-    <row r="67" spans="1:6" ht="35.25" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -2165,7 +2135,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
     </row>
-    <row r="68" spans="1:6" ht="35.25" customHeight="1">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -2173,7 +2143,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
     </row>
-    <row r="69" spans="1:6" ht="35.25" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -2181,7 +2151,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" ht="35.25" customHeight="1">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -2189,7 +2159,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="1:6" ht="35.25" customHeight="1">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -2197,7 +2167,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
     </row>
-    <row r="72" spans="1:6" ht="35.25" customHeight="1">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -2205,7 +2175,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="1:6" ht="35.25" customHeight="1">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -2213,7 +2183,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
     </row>
-    <row r="74" spans="1:6" ht="35.25" customHeight="1">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -2221,7 +2191,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
     </row>
-    <row r="75" spans="1:6" ht="35.25" customHeight="1">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -2229,7 +2199,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
-    <row r="76" spans="1:6" ht="35.25" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -2237,7 +2207,7 @@
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
     </row>
-    <row r="77" spans="1:6" ht="35.25" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -2245,7 +2215,7 @@
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
     </row>
-    <row r="78" spans="1:6" ht="35.25" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -2254,16 +2224,16 @@
       <c r="F78" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B10 B19 B21:B1010" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B10 B19 B21:B1010" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2271,20 +2241,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1">
+    <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32.25" customHeight="1">
+    <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2320,404 +2294,387 @@
       <c r="C2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="F3" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="13">
+      <c r="F2" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12"/>
-      <c r="F4" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="13">
+      <c r="F4" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12"/>
-      <c r="F5" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="38">
+      <c r="F5" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="39">
-      <c r="A7" s="14" t="s">
+      <c r="D6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26">
-      <c r="A8" s="15" t="s">
+      <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" ht="26">
-      <c r="A9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="F9" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="F10" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="65">
-      <c r="A11" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="3">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="13">
+      <c r="F11" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
-      <c r="F12" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="F13" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
-      <c r="F14" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="39">
-      <c r="A15" s="14" t="s">
-        <v>41</v>
+      <c r="F14" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="F15" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="39">
-      <c r="A16" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="26">
-      <c r="A17" s="15" t="s">
+      <c r="B17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="F17" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="F17" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="39">
-      <c r="A18" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12"/>
+      <c r="F19" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="9">
-        <v>2</v>
-      </c>
-      <c r="F18" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="13">
-      <c r="A19" s="12"/>
-      <c r="F19" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="26">
-      <c r="A20" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12"/>
+      <c r="F21" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="F20" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="13">
-      <c r="A21" s="12"/>
-      <c r="F21" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="52">
-      <c r="A22" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12"/>
+      <c r="F23" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="F22" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="13">
-      <c r="A23" s="12"/>
-      <c r="F23" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="26">
-      <c r="A24" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12"/>
+      <c r="F25" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9"/>
+      <c r="F26" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12"/>
+      <c r="F27" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12"/>
+      <c r="F28" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="13">
-      <c r="A25" s="12"/>
-      <c r="F25" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="9"/>
-      <c r="F26" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="13">
-      <c r="A27" s="12"/>
-      <c r="F27" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="13">
-      <c r="A28" s="12"/>
-      <c r="F28" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="13">
-      <c r="A29" s="12"/>
-      <c r="F29" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="25.5">
-      <c r="A30" s="13" t="s">
+      <c r="B30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="F30" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="13">
-      <c r="A31" s="12" t="s">
+      <c r="B31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="9" t="s">
+      <c r="F31" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="26">
-      <c r="A32" s="12" t="s">
+      <c r="B32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="F32" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="F32" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="38">
-      <c r="A33" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="51">
-      <c r="A34" s="12" t="s">
+      <c r="B34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="11" t="b">
-        <f>TRUE()</f>
+      <c r="F34" s="11" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1034" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B7 B9:B28 B30:B1034" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>